<commit_message>
Agregado el load de Pesos en Kaggle - Cargando datos de los modelos
</commit_message>
<xml_diff>
--- a/Models/Models.xlsx
+++ b/Models/Models.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB7BAA3-EB93-425C-B8CD-0420AD11C292}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6719679C-8FF7-45BD-87C9-FDF5EBBC09CE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Modelos" sheetId="1" r:id="rId1"/>
+    <sheet name="Paramétros" sheetId="2" r:id="rId1"/>
+    <sheet name="Modelos" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Accuracy - Train</t>
   </si>
@@ -52,17 +53,94 @@
     <t>Accuracy - Validation</t>
   </si>
   <si>
-    <t>Score - Validation</t>
-  </si>
-  <si>
     <t>Batch Size</t>
+  </si>
+  <si>
+    <t>MLP</t>
+  </si>
+  <si>
+    <t>CNN</t>
+  </si>
+  <si>
+    <t>CNN - 2 Layers + Dropout</t>
+  </si>
+  <si>
+    <t>CNN - 3 Layers + Dropout</t>
+  </si>
+  <si>
+    <t>SimpleRNN + Dropout</t>
+  </si>
+  <si>
+    <t>LSTM + Dropout</t>
+  </si>
+  <si>
+    <t>GRU + Dropout</t>
+  </si>
+  <si>
+    <t>2 layers CNN - LSTM + Dropout</t>
+  </si>
+  <si>
+    <t>LSTM - 2 layers CNN+ Dropout</t>
+  </si>
+  <si>
+    <t>CNN-RNN model with Concatenate and Dropout</t>
+  </si>
+  <si>
+    <t>CNN-RNN-MLP model with Concatenate and Dropout</t>
+  </si>
+  <si>
+    <t>Multilayer - CNN - RNN model - Strides</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>Fasttext supervised</t>
+  </si>
+  <si>
+    <t>ADAM</t>
+  </si>
+  <si>
+    <t>Loss - Validation</t>
+  </si>
+  <si>
+    <t>Paramétros</t>
+  </si>
+  <si>
+    <t>Valores</t>
+  </si>
+  <si>
+    <t>Max_Features</t>
+  </si>
+  <si>
+    <t>Max_Length</t>
+  </si>
+  <si>
+    <t>Validation_Size</t>
+  </si>
+  <si>
+    <t>Embedding_Size</t>
+  </si>
+  <si>
+    <t>Training Dataset Size</t>
+  </si>
+  <si>
+    <t>Testing Dataset Size</t>
+  </si>
+  <si>
+    <t>Validation Dataset Size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="169" formatCode="#,##0.0"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="172" formatCode="#,##0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,16 +148,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,17 +183,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Énfasis2" xfId="1" builtinId="33"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -111,15 +264,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF1620C6-9B8C-45DF-8C23-190529A17884}" name="Tabla1" displayName="Tabla1" ref="A1:L17" totalsRowShown="0">
-  <autoFilter ref="A1:L17" xr:uid="{79EBDBBE-D7AF-4644-A9EF-17886CD8F74E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8B5E8124-4160-46B9-956A-8230CC28C4F4}" name="Tabla3" displayName="Tabla3" ref="A1:B7" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
+  <autoFilter ref="A1:B7" xr:uid="{B620053E-EE78-4C50-9D19-56DC1188108F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{DC9F3A8F-2EF4-45C6-98B0-A9C3871B4997}" name="Paramétros" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{F729E600-6304-4505-8B80-D553E1D9B396}" name="Valores" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF1620C6-9B8C-45DF-8C23-190529A17884}" name="Tabla1" displayName="Tabla1" ref="A1:L16" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:L16" xr:uid="{79EBDBBE-D7AF-4644-A9EF-17886CD8F74E}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{4E4B7A70-6426-4F2C-87D3-B6F7197204B2}" name="Model"/>
     <tableColumn id="9" xr3:uid="{88400789-B17A-4A54-A8F9-70B764CA83D9}" name="Parameters"/>
     <tableColumn id="2" xr3:uid="{C5956042-B419-405F-922E-48AD14156BBA}" name="Accuracy - Train"/>
     <tableColumn id="3" xr3:uid="{6ED152AC-FE8B-4B34-8E7A-98A8731A5BED}" name="Loss - Train"/>
     <tableColumn id="10" xr3:uid="{9A00BA4F-FA95-4326-B812-212B916FAAED}" name="Accuracy - Validation"/>
-    <tableColumn id="11" xr3:uid="{64EE56FD-0350-4D20-8571-A4CE187F6913}" name="Score - Validation"/>
+    <tableColumn id="11" xr3:uid="{64EE56FD-0350-4D20-8571-A4CE187F6913}" name="Loss - Validation"/>
     <tableColumn id="4" xr3:uid="{2B0F85DA-A443-4D84-8562-1F05FEE67DEA}" name="Accuracy - Test"/>
     <tableColumn id="5" xr3:uid="{D6DD238E-D4AC-48BC-8814-B644623DF29D}" name="Score - Test"/>
     <tableColumn id="6" xr3:uid="{E2A10B7F-EC24-4FB1-A53B-EED664BA6325}" name="Learning Rate"/>
@@ -393,64 +557,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2663BD0-1F66-4864-81E0-3FA8E24E1B3D}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" t="s">
-        <v>3</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="5">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="5">
+        <v>128</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="5">
+        <f>E5*(1-E4)</f>
+        <v>2880000</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3600000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="5">
+        <f>E5*E4</f>
+        <v>720000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="5">
+        <v>400000</v>
       </c>
     </row>
   </sheetData>
@@ -459,4 +647,473 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="C4:H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2589313</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.90590000000000004</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0.23960000000000001</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0.90324000000000004</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0.24660000000000001</v>
+      </c>
+      <c r="G2" s="9">
+        <v>0.90231999996185297</v>
+      </c>
+      <c r="H2" s="9">
+        <v>0.24728829448699899</v>
+      </c>
+      <c r="I2" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1024</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2651137</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.92749999999999999</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.19009999999999999</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0.9234</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0.92315749996185303</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.20039440320014901</v>
+      </c>
+      <c r="I3" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1024</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2814721</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.93910000000000005</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.16250000000000001</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.93579999999999997</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0.93540249998092595</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.17181611125469201</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1024</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2900481</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1024</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2658817</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1024</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2955521</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1024</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2856705</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1024</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3316481</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1024</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="5">
+        <v>3308289</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1024</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="5">
+        <v>4902401</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1024</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="5">
+        <v>9805313</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1024</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="5">
+        <v>7911041</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.94610000000000005</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.14829999999999999</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0.93820000000000003</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0.1663</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0.93711249998092605</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0.168645723261833</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1024</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>